<commit_message>
comitting GB entity files - Shipra Task
</commit_message>
<xml_diff>
--- a/src/test/resources/com/sirion/xls/Governance Body Suite.xlsx
+++ b/src/test/resources/com/sirion/xls/Governance Body Suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="60">
   <si>
     <t>TCID</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t>Gbworkflow</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>GBUpdate</t>
@@ -602,7 +599,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,9 +638,11 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -653,16 +652,16 @@
         <v>55</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
@@ -693,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" workbookViewId="0">
-      <selection sqref="A1:AJ2"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +728,7 @@
     <col min="30" max="30" customWidth="true" width="27.28515625" collapsed="true"/>
     <col min="31" max="31" customWidth="true" width="18.0" collapsed="true"/>
     <col min="32" max="33" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="7.48828125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -904,10 +903,10 @@
         <v>2017</v>
       </c>
       <c r="X2" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y2" s="5">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="Z2" s="5">
         <v>2017</v>
@@ -934,7 +933,7 @@
         <v>4</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="AJ2" s="5"/>
     </row>
@@ -948,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,10 +977,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>

</xml_diff>